<commit_message>
change constant in framerate calculator
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -608,7 +608,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,11 +716,11 @@
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>5.36</v>
+        <v>5.4</v>
       </c>
       <c r="C11" s="3">
         <f>B11*0.000001</f>
-        <v>5.3600000000000004E-6</v>
+        <v>5.4E-6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
       </c>
       <c r="B19" s="13">
         <f>(C8*(3+B15+1+B7+7+7)-C14+C9+C10+C11)/0.000001</f>
-        <v>35367.510000000009</v>
+        <v>35367.550000000003</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Timings pour XGS5000, framerate calculator
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="14355"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="14355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="XGS12000" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="XGS5000" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>SensorPeriodNanoSecond</t>
   </si>
@@ -54,9 +54,6 @@
     <t>EXP_FOT(us)</t>
   </si>
   <si>
-    <t>Trig_2_EXP(us)</t>
-  </si>
-  <si>
     <t>Estimated Exposure Max</t>
   </si>
   <si>
@@ -76,6 +73,21 @@
   </si>
   <si>
     <t xml:space="preserve"> (wip: 17021)</t>
+  </si>
+  <si>
+    <t>XGS5000 Framerate calculator</t>
+  </si>
+  <si>
+    <t>FOTn_2_EXP(us)</t>
+  </si>
+  <si>
+    <t>* From internal FOT(multiple nb lines)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (wip: 17175)</t>
+  </si>
+  <si>
+    <t>Y_SIZE(lines,max)</t>
   </si>
 </sst>
 </file>
@@ -605,9 +617,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -618,21 +630,21 @@
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -643,7 +655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -652,7 +664,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -661,21 +673,21 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4">
         <v>3072</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -687,7 +699,7 @@
         <v>1.14375E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -699,7 +711,7 @@
         <v>5.1199999999999998E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -711,7 +723,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -723,7 +735,7 @@
         <v>5.4E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -732,7 +744,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -741,9 +753,9 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B14" s="8">
         <v>76.8</v>
@@ -752,17 +764,20 @@
         <f>B14*0.000001</f>
         <v>7.6799999999999997E-5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="10">
         <v>2</v>
       </c>
       <c r="C15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -774,26 +789,26 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5">
         <f>1/(C9+C10+(C8*(B12+3+B13+1+B7+7+7)))</f>
         <v>28.126764514992619</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="13">
         <f>(C8*(3+B15+1+B7+7+7)-C14+C9+C10+C11)/0.000001</f>
         <v>35367.550000000003</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -814,12 +829,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15.625</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2048</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>732</v>
+      </c>
+      <c r="C8" s="2">
+        <f>B8 *B4*0.000000001</f>
+        <v>1.14375E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="C9" s="3">
+        <f>B9*0.000001</f>
+        <v>5.1199999999999998E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2">
+        <f>B10*0.000001</f>
+        <v>2.3E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <f>B11*0.000001</f>
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8">
+        <v>76.8</v>
+      </c>
+      <c r="C14" s="8">
+        <f>B14*0.000001</f>
+        <v>7.6799999999999997E-5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <v>2</v>
+      </c>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5">
+        <f>1/(C9+C10+(C8*(B12+3+B13+1+B7+7+7)))</f>
+        <v>41.943977526416845</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="13">
+        <f>(C8*(3+B15+1+B7+7+7)-C14+C9+C10+C11)/0.000001</f>
+        <v>23657.15</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Modifications a la feuille de calcul fps XGS avec XGS8000
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="14355" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="14355"/>
   </bookViews>
   <sheets>
     <sheet name="XGS12000" sheetId="1" r:id="rId1"/>
     <sheet name="XGS5000" sheetId="2" r:id="rId2"/>
     <sheet name="XGS16000" sheetId="3" r:id="rId3"/>
+    <sheet name="XGS8000" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
   <si>
     <t>SensorPeriodNanoSecond</t>
   </si>
@@ -69,31 +70,52 @@
     <t>fps</t>
   </si>
   <si>
-    <t>Y_SIZE(lines, 3072 max)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (wip: 17021)</t>
   </si>
   <si>
     <t>XGS5000 Framerate calculator</t>
   </si>
   <si>
-    <t>FOTn_2_EXP(us)</t>
-  </si>
-  <si>
-    <t>* From internal FOT(multiple nb lines)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> (wip: 17175)</t>
   </si>
   <si>
-    <t>Y_SIZE(lines,max)</t>
-  </si>
-  <si>
     <t>XGS16000 Framerate calculator</t>
   </si>
   <si>
     <t xml:space="preserve"> (wip: 17169)</t>
+  </si>
+  <si>
+    <t>XGS8000 Framerate calculator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (wip: 18093)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full surface XY with Y Inperpol. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y_SIZE with Interpolation </t>
+  </si>
+  <si>
+    <t>Y_SIZE ROI(lines, 2056 max)</t>
+  </si>
+  <si>
+    <t>Y_SIZE ROI(lines, 3080 max)</t>
+  </si>
+  <si>
+    <t>Y_SIZE ROI(lines, 4008 max)</t>
+  </si>
+  <si>
+    <t>Y_SIZE ROI(lines, 2168 max)</t>
+  </si>
+  <si>
+    <t>ROI Estimated Framerate Max</t>
+  </si>
+  <si>
+    <t>ROI Estimated Exposure Max</t>
+  </si>
+  <si>
+    <t>FOTn_2_EXP(us) (int FOT nb line)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +193,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -288,11 +322,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -316,6 +396,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,34 +720,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -661,132 +758,133 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="8">
         <v>15.625</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="25">
         <v>16</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="31">
+        <v>3080</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="30">
         <v>3072</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>732</v>
       </c>
-      <c r="C8" s="2">
-        <f>B8 *B4*0.000000001</f>
+      <c r="C9" s="2">
+        <f>B9 *B4*0.000000001</f>
         <v>1.14375E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <v>51.2</v>
       </c>
-      <c r="C9" s="3">
-        <f>B9*0.000001</f>
+      <c r="C10" s="3">
+        <f>B10*0.000001</f>
         <v>5.1199999999999998E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>23</v>
       </c>
-      <c r="C10" s="2">
-        <f>B10*0.000001</f>
+      <c r="C11" s="2">
+        <f>B11*0.000001</f>
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <v>5.4</v>
       </c>
-      <c r="C11" s="3">
-        <f>B11*0.000001</f>
+      <c r="C12" s="3">
+        <f>B12*0.000001</f>
         <v>5.4E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>2</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="8">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8">
         <v>76.8</v>
       </c>
-      <c r="C14" s="8">
-        <f>B14*0.000001</f>
+      <c r="C15" s="8">
+        <f>B15*0.000001</f>
         <v>7.6799999999999997E-5</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B16" s="10">
         <v>2</v>
       </c>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -794,34 +892,46 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="5">
-        <f>1/(C9+C10+(C8*(B12+3+B13+1+B7+7+7)))</f>
-        <v>28.126764514992619</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
+        <v>28.054563320201456</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="13">
-        <f>(C8*(3+B15+1+B7+7+7)-C14+C9+C10+C11)/0.000001</f>
+        <v>30</v>
+      </c>
+      <c r="B19" s="5">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
+        <v>28.126764514992619</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="13">
+        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
         <v>35367.550000000003</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+    <row r="25" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -835,33 +945,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C20"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -872,132 +983,133 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="8">
         <v>15.625</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="25">
         <v>16</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="31">
+        <v>2056</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="30">
+        <v>2048</v>
+      </c>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>732</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B9 *B4*0.000000001</f>
+        <v>1.14375E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="C10" s="3">
+        <f>B10*0.000001</f>
+        <v>5.1199999999999998E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
         <v>23</v>
       </c>
-      <c r="B7" s="4">
-        <v>2048</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>732</v>
-      </c>
-      <c r="C8" s="2">
-        <f>B8 *B4*0.000000001</f>
-        <v>1.14375E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>51.2</v>
-      </c>
-      <c r="C9" s="3">
-        <f>B9*0.000001</f>
-        <v>5.1199999999999998E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2">
-        <f>B10*0.000001</f>
+      <c r="C11" s="2">
+        <f>B11*0.000001</f>
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="3">
-        <f>B11*0.000001</f>
+      <c r="C12" s="3">
+        <f>B12*0.000001</f>
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>2</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="8">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8">
         <v>76.8</v>
       </c>
-      <c r="C14" s="8">
-        <f>B14*0.000001</f>
+      <c r="C15" s="8">
+        <f>B15*0.000001</f>
         <v>7.6799999999999997E-5</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B16" s="10">
         <v>2</v>
       </c>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -1005,26 +1117,38 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="5">
-        <f>1/(C9+C10+(C8*(B12+3+B13+1+B7+7+7)))</f>
-        <v>41.943977526416845</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
+        <v>41.783617270422525</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
+        <v>41.943977526416845</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="13">
-        <f>(C8*(3+B15+1+B7+7+7)-C14+C9+C10+C11)/0.000001</f>
+      <c r="B20" s="13">
+        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
         <v>23657.15</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1039,31 +1163,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="A1" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1077,128 +1202,132 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="8">
         <v>15.625</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="25">
         <v>16</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="31">
+        <v>4008</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="30">
+        <v>4000</v>
+      </c>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>732</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B9 *B4*0.000000001</f>
+        <v>1.14375E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="C10" s="3">
+        <f>B10*0.000001</f>
+        <v>5.1199999999999998E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
         <v>23</v>
       </c>
-      <c r="B7" s="4">
-        <v>4000</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>732</v>
-      </c>
-      <c r="C8" s="2">
-        <f>B8 *B4*0.000000001</f>
-        <v>1.14375E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
-        <v>51.2</v>
-      </c>
-      <c r="C9" s="3">
-        <f>B9*0.000001</f>
-        <v>5.1199999999999998E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2">
-        <f>B10*0.000001</f>
+      <c r="C11" s="2">
+        <f>B11*0.000001</f>
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <v>7.12</v>
       </c>
-      <c r="C11" s="3">
-        <f>B11*0.000001</f>
+      <c r="C12" s="3">
+        <f>B12*0.000001</f>
         <v>7.1199999999999996E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>2</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="8">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8">
         <v>76.8</v>
       </c>
-      <c r="C14" s="8">
-        <f>B14*0.000001</f>
+      <c r="C15" s="8">
+        <f>B15*0.000001</f>
         <v>7.6799999999999997E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B16" s="10">
         <v>2</v>
       </c>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -1206,26 +1335,38 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="5">
-        <f>1/(C9+C10+(C8*(B12+3+B13+1+B7+7+7)))</f>
-        <v>21.660340944596637</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
+        <v>21.617496769535325</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
+        <v>21.660340944596637</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="13">
-        <f>(C8*(3+B15+1+B7+7+7)-C14+C9+C10+C11)/0.000001</f>
+      <c r="B20" s="13">
+        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
         <v>45983.270000000004</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1236,4 +1377,223 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15.625</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="24">
+        <v>16</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="26">
+        <v>2168</v>
+      </c>
+      <c r="C7" s="28"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2160</v>
+      </c>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>732</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B9 *B4*0.000000001</f>
+        <v>1.14375E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="C10" s="3">
+        <f>B10*0.000001</f>
+        <v>5.1199999999999998E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11*0.000001</f>
+        <v>2.3E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="C12" s="3">
+        <f>B12*0.000001</f>
+        <v>5.4E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8">
+        <v>76.8</v>
+      </c>
+      <c r="C15" s="8">
+        <f>B15*0.000001</f>
+        <v>7.6799999999999997E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
+        <v>39.660781337222737</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
+        <v>39.805232994955681</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="13">
+        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
+        <v>24936.550000000003</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix ONSEMI initialistion code Fix for load dcf XGS2000 v2 Add framerate calculator for XGS2000 Add validation waveforms for XGS2000
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="14355"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="14355" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="XGS12000" sheetId="1" r:id="rId1"/>
-    <sheet name="XGS5000" sheetId="2" r:id="rId2"/>
-    <sheet name="XGS16000" sheetId="3" r:id="rId3"/>
-    <sheet name="XGS8000" sheetId="4" r:id="rId4"/>
+    <sheet name="XGS8000" sheetId="4" r:id="rId2"/>
+    <sheet name="XGS5000" sheetId="2" r:id="rId3"/>
+    <sheet name="XGS2000" sheetId="5" r:id="rId4"/>
+    <sheet name="XGS16000" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="33">
   <si>
     <t>SensorPeriodNanoSecond</t>
   </si>
@@ -722,7 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -948,7 +949,226 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15.625</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="24">
+        <v>16</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="26">
+        <v>2168</v>
+      </c>
+      <c r="C7" s="28"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2160</v>
+      </c>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>732</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B9 *B4*0.000000001</f>
+        <v>1.14375E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="C10" s="3">
+        <f>B10*0.000001</f>
+        <v>5.1199999999999998E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11*0.000001</f>
+        <v>2.3E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="C12" s="3">
+        <f>B12*0.000001</f>
+        <v>5.4E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8">
+        <v>76.8</v>
+      </c>
+      <c r="C15" s="8">
+        <f>B15*0.000001</f>
+        <v>7.6799999999999997E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
+        <v>39.660781337222737</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
+        <v>39.805232994955681</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="13">
+        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
+        <v>24936.550000000003</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1381,225 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>15.625</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25">
+        <v>16</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="31">
+        <v>1208</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="30">
+        <v>1200</v>
+      </c>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>732</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B9 *B4*0.000000001</f>
+        <v>1.14375E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="C10" s="3">
+        <f>B10*0.000001</f>
+        <v>5.1199999999999998E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11*0.000001</f>
+        <v>2.3E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <f>B12*0.000001</f>
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8">
+        <v>76.8</v>
+      </c>
+      <c r="C15" s="8">
+        <f>B15*0.000001</f>
+        <v>7.6799999999999997E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
+        <v>70.255184393513332</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
+        <v>70.709731249988948</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="13">
+        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
+        <v>13958.150000000001</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -1377,223 +1815,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2">
-        <v>15.625</v>
-      </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="24">
-        <v>16</v>
-      </c>
-      <c r="C5" s="25"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="26">
-        <v>2168</v>
-      </c>
-      <c r="C7" s="28"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4">
-        <v>2160</v>
-      </c>
-      <c r="C8" s="27"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>732</v>
-      </c>
-      <c r="C9" s="2">
-        <f>B9 *B4*0.000000001</f>
-        <v>1.14375E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3">
-        <v>51.2</v>
-      </c>
-      <c r="C10" s="3">
-        <f>B10*0.000001</f>
-        <v>5.1199999999999998E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2">
-        <f>B11*0.000001</f>
-        <v>2.3E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="C12" s="3">
-        <f>B12*0.000001</f>
-        <v>5.4E-6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="8">
-        <v>76.8</v>
-      </c>
-      <c r="C15" s="8">
-        <f>B15*0.000001</f>
-        <v>7.6799999999999997E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="10">
-        <v>2</v>
-      </c>
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="17">
-        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
-        <v>39.660781337222737</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="5">
-        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
-        <v>39.805232994955681</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="13">
-        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
-        <v>24936.550000000003</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add missing files :)
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -14,11 +14,12 @@
     <sheet name="XGS16000" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="37">
   <si>
     <t>SensorPeriodNanoSecond</t>
   </si>
@@ -123,6 +124,12 @@
   </si>
   <si>
     <t xml:space="preserve"> (wip: 18248)</t>
+  </si>
+  <si>
+    <t>XGS5000 COLOR Framerate calculator</t>
+  </si>
+  <si>
+    <t>XGS12000 COLOR Framerate calculator</t>
   </si>
 </sst>
 </file>
@@ -716,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,10 +930,207 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7">
+        <v>15.625</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="23">
+        <v>16</v>
+      </c>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="29">
+        <v>3080</v>
+      </c>
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="28">
+        <v>3072</v>
+      </c>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <f>732*4</f>
+        <v>2928</v>
+      </c>
+      <c r="C32" s="2">
+        <f>B32 *B27*0.000000001</f>
+        <v>4.5750000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3">
+        <v>188</v>
+      </c>
+      <c r="C33" s="3">
+        <f>B33*0.000001</f>
+        <v>1.8799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
+        <v>91.6</v>
+      </c>
+      <c r="C34" s="2">
+        <f>B34*0.000001</f>
+        <v>9.159999999999999E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="C35" s="3">
+        <f>B35*0.000001</f>
+        <v>5.4E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="7">
+        <v>213.6</v>
+      </c>
+      <c r="C38" s="7">
+        <f>B38*0.000001</f>
+        <v>2.1359999999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="15">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
+        <v>7.0144870200424938</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+7+7)))</f>
+        <v>7.0325416801164033</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="12">
+        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>141530.39999999997</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1154,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C20"/>
+      <selection activeCell="A24" sqref="A24:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,10 +1565,206 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7">
+        <v>15.625</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="23">
+        <v>16</v>
+      </c>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="29">
+        <v>2056</v>
+      </c>
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="28">
+        <v>2048</v>
+      </c>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2928</v>
+      </c>
+      <c r="C32" s="2">
+        <f>B32 *B27*0.000000001</f>
+        <v>4.5750000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3">
+        <v>188</v>
+      </c>
+      <c r="C33" s="3">
+        <f>B33*0.000001</f>
+        <v>1.8799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
+        <v>91.2</v>
+      </c>
+      <c r="C34" s="2">
+        <f>B34*0.000001</f>
+        <v>9.1199999999999994E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3">
+        <f>B35*0.000001</f>
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="7">
+        <v>213.6</v>
+      </c>
+      <c r="C38" s="7">
+        <f>B38*0.000001</f>
+        <v>2.1359999999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="15">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
+        <v>10.44782512848213</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+7+7)))</f>
+        <v>10.487929965798861</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="12">
+        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>94683.599999999991</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated XGS excel FPS calculator
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="27555" windowHeight="14355"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="24405" windowHeight="14355" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="XGS12000" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="XGS16000" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="40">
   <si>
     <t>SensorPeriodNanoSecond</t>
   </si>
@@ -130,6 +129,15 @@
   </si>
   <si>
     <t>XGS12000 COLOR Framerate calculator</t>
+  </si>
+  <si>
+    <t>XGS8000C Framerate calculator</t>
+  </si>
+  <si>
+    <t>Y Line Color Interpolation</t>
+  </si>
+  <si>
+    <t>XGS2000C Framerate calculator</t>
   </si>
 </sst>
 </file>
@@ -723,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,43 +1093,52 @@
       <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
+      <c r="A40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="9">
+        <v>4</v>
+      </c>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B42" s="15">
         <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
         <v>7.0144870200424938</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="5">
-        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+7+7)))</f>
-        <v>7.0325416801164033</v>
-      </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
+        <v>7.0235027472431009</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B44" s="12">
         <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
         <v>141530.39999999997</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C44" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1139,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,10 +1363,216 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
+        <v>15.625</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="22">
+        <v>16</v>
+      </c>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="24">
+        <v>2168</v>
+      </c>
+      <c r="C30" s="26"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2160</v>
+      </c>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <f>732*4</f>
+        <v>2928</v>
+      </c>
+      <c r="C32" s="2">
+        <f>B32 *B27*0.000000001</f>
+        <v>4.5750000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3">
+        <v>188</v>
+      </c>
+      <c r="C33" s="3">
+        <f>B33*0.000001</f>
+        <v>1.8799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
+        <v>91.6</v>
+      </c>
+      <c r="C34" s="2">
+        <f>B34*0.000001</f>
+        <v>9.159999999999999E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="C35" s="3">
+        <f>B35*0.000001</f>
+        <v>5.4E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="7">
+        <v>213.6</v>
+      </c>
+      <c r="C38" s="7">
+        <f>B38*0.000001</f>
+        <v>2.1359999999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="9">
+        <v>4</v>
+      </c>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="15">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
+        <v>9.9168865736264369</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
+        <v>9.9349163629065984</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="12">
+        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>99806.400000000009</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1358,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C43"/>
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,43 +1942,52 @@
       <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
+      <c r="A40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="9">
+        <v>4</v>
+      </c>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B42" s="15">
         <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
         <v>10.44782512848213</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="5">
-        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+7+7)))</f>
-        <v>10.487929965798861</v>
-      </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
+        <v>10.467839134435318</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B44" s="12">
         <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
         <v>94683.599999999991</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C44" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1772,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,10 +2211,216 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7">
+        <v>15.625</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="23">
+        <v>16</v>
+      </c>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="29">
+        <v>1208</v>
+      </c>
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="28">
+        <v>1200</v>
+      </c>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <f>732*4</f>
+        <v>2928</v>
+      </c>
+      <c r="C32" s="2">
+        <f>B32 *B27*0.000000001</f>
+        <v>4.5750000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3">
+        <v>188.4</v>
+      </c>
+      <c r="C33" s="3">
+        <f>B33*0.000001</f>
+        <v>1.884E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
+        <v>91.2</v>
+      </c>
+      <c r="C34" s="2">
+        <f>B34*0.000001</f>
+        <v>9.1199999999999994E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3">
+        <f>B35*0.000001</f>
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="7">
+        <v>213.6</v>
+      </c>
+      <c r="C38" s="7">
+        <f>B38*0.000001</f>
+        <v>2.1359999999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="9">
+        <v>4</v>
+      </c>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="15">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
+        <v>17.56910367703771</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
+        <v>17.625773110473059</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="12">
+        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>55888</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add xgs new ini files XGS12000C corrected ReadOutN_2_TrigN(us) in spread sheet
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="345" windowWidth="24405" windowHeight="14355" activeTab="3"/>
+    <workbookView xWindow="720" yWindow="345" windowWidth="24405" windowHeight="14355"/>
   </bookViews>
   <sheets>
     <sheet name="XGS12000" sheetId="1" r:id="rId1"/>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,11 +1022,11 @@
         <v>3</v>
       </c>
       <c r="B33" s="3">
-        <v>188</v>
+        <v>188.4</v>
       </c>
       <c r="C33" s="3">
         <f>B33*0.000001</f>
-        <v>1.8799999999999999E-4</v>
+        <v>1.884E-4</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="B42" s="15">
         <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
-        <v>7.0144870200424938</v>
+        <v>7.0144673388864529</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>16</v>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="B43" s="5">
         <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
-        <v>7.0235027472431009</v>
+        <v>7.0234830154621983</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>16</v>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B44" s="12">
         <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
-        <v>141530.39999999997</v>
+        <v>141530.79999999999</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>15</v>
@@ -2006,7 +2006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add excel framerate calculator for XGS 16000 Color
</commit_message>
<xml_diff>
--- a/athena/bench/XGS_FrameRate_Calc.xlsx
+++ b/athena/bench/XGS_FrameRate_Calc.xlsx
@@ -7,18 +7,18 @@
     <workbookView xWindow="720" yWindow="345" windowWidth="24405" windowHeight="14355"/>
   </bookViews>
   <sheets>
-    <sheet name="XGS12000" sheetId="1" r:id="rId1"/>
-    <sheet name="XGS8000" sheetId="4" r:id="rId2"/>
-    <sheet name="XGS5000" sheetId="2" r:id="rId3"/>
-    <sheet name="XGS2000" sheetId="5" r:id="rId4"/>
-    <sheet name="XGS16000" sheetId="3" r:id="rId5"/>
+    <sheet name="XGS16000" sheetId="3" r:id="rId1"/>
+    <sheet name="XGS12000" sheetId="1" r:id="rId2"/>
+    <sheet name="XGS8000" sheetId="4" r:id="rId3"/>
+    <sheet name="XGS5000" sheetId="2" r:id="rId4"/>
+    <sheet name="XGS2000" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="42">
   <si>
     <t>SensorPeriodNanoSecond</t>
   </si>
@@ -131,13 +131,19 @@
     <t>XGS12000 COLOR Framerate calculator</t>
   </si>
   <si>
-    <t>XGS8000C Framerate calculator</t>
-  </si>
-  <si>
     <t>Y Line Color Interpolation</t>
   </si>
   <si>
-    <t>XGS2000C Framerate calculator</t>
+    <t>XGS16000 COLOR Framerate calculator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (wip: 18963)</t>
+  </si>
+  <si>
+    <t>XGS8000 COLOR Framerate calculator</t>
+  </si>
+  <si>
+    <t>XGS2000 COLOR Framerate calculator</t>
   </si>
 </sst>
 </file>
@@ -733,8 +739,433 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7">
+        <v>15.625</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="23">
+        <v>16</v>
+      </c>
+      <c r="C5" s="23"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="29">
+        <v>4008</v>
+      </c>
+      <c r="C7" s="23"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="28">
+        <v>4000</v>
+      </c>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>732</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B9 *B4*0.000000001</f>
+        <v>1.14375E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="C10" s="3">
+        <f>B10*0.000001</f>
+        <v>5.1199999999999998E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11*0.000001</f>
+        <v>2.3E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7.12</v>
+      </c>
+      <c r="C12" s="3">
+        <f>B12*0.000001</f>
+        <v>7.1199999999999996E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="7">
+        <v>76.8</v>
+      </c>
+      <c r="C15" s="7">
+        <f>B15*0.000001</f>
+        <v>7.6799999999999997E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="15">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
+        <v>21.617496769535325</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="5">
+        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
+        <v>21.660340944596637</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="12">
+        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
+        <v>45983.270000000004</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7">
+        <v>15.625</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="23">
+        <v>16</v>
+      </c>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="29">
+        <v>4008</v>
+      </c>
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="28">
+        <v>4000</v>
+      </c>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <f>732*4</f>
+        <v>2928</v>
+      </c>
+      <c r="C32" s="2">
+        <f>B32 *B27*0.000000001</f>
+        <v>4.5750000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3">
+        <v>188</v>
+      </c>
+      <c r="C33" s="3">
+        <f>B33*0.000001</f>
+        <v>1.8799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
+        <v>91.6</v>
+      </c>
+      <c r="C34" s="2">
+        <f>B34*0.000001</f>
+        <v>9.159999999999999E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="C35" s="3">
+        <f>B35*0.000001</f>
+        <v>7.0999999999999989E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="7">
+        <v>214</v>
+      </c>
+      <c r="C38" s="7">
+        <f>B38*0.000001</f>
+        <v>2.14E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="9">
+        <v>4</v>
+      </c>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="15">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
+        <v>5.4048766039646932</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
+        <v>5.410227819283242</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="12">
+        <f>(C32*(3+B39+1+B31+B40+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>184170.70000000004</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1525,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="9">
         <v>4</v>
@@ -1135,8 +1566,8 @@
         <v>31</v>
       </c>
       <c r="B44" s="12">
-        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
-        <v>141530.79999999999</v>
+        <f>(C32*(3+B39+1+B31+B40+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>141713.79999999999</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>15</v>
@@ -1154,12 +1585,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D44" sqref="D43:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1796,7 @@
     </row>
     <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
@@ -1519,7 +1950,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="9">
         <v>4</v>
@@ -1560,8 +1991,8 @@
         <v>12</v>
       </c>
       <c r="B44" s="12">
-        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
-        <v>99806.400000000009</v>
+        <f>(C32*(3+B39+1+B31+B40+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>99989.400000000009</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>15</v>
@@ -1579,12 +2010,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+      <selection activeCell="D43" sqref="D43:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,7 +2374,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="9">
         <v>4</v>
@@ -1984,432 +2415,8 @@
         <v>12</v>
       </c>
       <c r="B44" s="12">
-        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
-        <v>94683.599999999991</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7">
-        <v>15.625</v>
-      </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="23">
-        <v>16</v>
-      </c>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="29">
-        <v>1208</v>
-      </c>
-      <c r="C7" s="23"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="28">
-        <v>1200</v>
-      </c>
-      <c r="C8" s="25"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>732</v>
-      </c>
-      <c r="C9" s="2">
-        <f>B9 *B4*0.000000001</f>
-        <v>1.14375E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3">
-        <v>51.2</v>
-      </c>
-      <c r="C10" s="3">
-        <f>B10*0.000001</f>
-        <v>5.1199999999999998E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2">
-        <f>B11*0.000001</f>
-        <v>2.3E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3">
-        <f>B12*0.000001</f>
-        <v>6.9999999999999999E-6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="7">
-        <v>76.8</v>
-      </c>
-      <c r="C15" s="7">
-        <f>B15*0.000001</f>
-        <v>7.6799999999999997E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="9">
-        <v>2</v>
-      </c>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="15">
-        <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
-        <v>70.255184393513332</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="5">
-        <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
-        <v>70.709731249988948</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="12">
-        <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
-        <v>13958.150000000001</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="7">
-        <v>15.625</v>
-      </c>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="23">
-        <v>16</v>
-      </c>
-      <c r="C28" s="23"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="29">
-        <v>1208</v>
-      </c>
-      <c r="C30" s="23"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="28">
-        <v>1200</v>
-      </c>
-      <c r="C31" s="25"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="2">
-        <f>732*4</f>
-        <v>2928</v>
-      </c>
-      <c r="C32" s="2">
-        <f>B32 *B27*0.000000001</f>
-        <v>4.5750000000000001E-5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="3">
-        <v>188.4</v>
-      </c>
-      <c r="C33" s="3">
-        <f>B33*0.000001</f>
-        <v>1.884E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="2">
-        <v>91.2</v>
-      </c>
-      <c r="C34" s="2">
-        <f>B34*0.000001</f>
-        <v>9.1199999999999994E-5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="3">
-        <v>7</v>
-      </c>
-      <c r="C35" s="3">
-        <f>B35*0.000001</f>
-        <v>6.9999999999999999E-6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="2">
-        <v>10</v>
-      </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="3">
-        <v>2</v>
-      </c>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="7">
-        <v>213.6</v>
-      </c>
-      <c r="C38" s="7">
-        <f>B38*0.000001</f>
-        <v>2.1359999999999999E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="9">
-        <v>2</v>
-      </c>
-      <c r="C39" s="10"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="9">
-        <v>4</v>
-      </c>
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="15">
-        <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
-        <v>17.56910367703771</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="5">
-        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
-        <v>17.625773110473059</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="12">
-        <f>(C32*(3+B39+1+B31+7+7)-C38+C33+C34+C35)/0.000001</f>
-        <v>55888</v>
+        <f>(C32*(3+B39+1+B31+B40+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>94866.6</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>15</v>
@@ -2428,29 +2435,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="D43" sqref="D43:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -2494,16 +2501,16 @@
         <v>25</v>
       </c>
       <c r="B7" s="29">
-        <v>4008</v>
+        <v>1208</v>
       </c>
       <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="28">
-        <v>4000</v>
+        <v>1200</v>
       </c>
       <c r="C8" s="25"/>
     </row>
@@ -2548,11 +2555,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>7.12</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3">
         <f>B12*0.000001</f>
-        <v>7.1199999999999996E-6</v>
+        <v>6.9999999999999999E-6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,7 +2612,7 @@
       </c>
       <c r="B18" s="15">
         <f>1/(C10+C11+(C9*(B13+3+B14+1+B7+7+7)))</f>
-        <v>21.617496769535325</v>
+        <v>70.255184393513332</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>16</v>
@@ -2617,7 +2624,7 @@
       </c>
       <c r="B19" s="5">
         <f>1/(C10+C11+(C9*(B13+3+B14+1+B8+7+7)))</f>
-        <v>21.660340944596637</v>
+        <v>70.709731249988948</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>16</v>
@@ -2629,16 +2636,222 @@
       </c>
       <c r="B20" s="12">
         <f>(C9*(3+B16+1+B8+7+7)-C15+C10+C11+C12)/0.000001</f>
-        <v>45983.270000000004</v>
+        <v>13958.150000000001</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7">
+        <v>15.625</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="23">
+        <v>16</v>
+      </c>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="29">
+        <v>1208</v>
+      </c>
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="28">
+        <v>1200</v>
+      </c>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <f>732*4</f>
+        <v>2928</v>
+      </c>
+      <c r="C32" s="2">
+        <f>B32 *B27*0.000000001</f>
+        <v>4.5750000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3">
+        <v>188.4</v>
+      </c>
+      <c r="C33" s="3">
+        <f>B33*0.000001</f>
+        <v>1.884E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
+        <v>91.2</v>
+      </c>
+      <c r="C34" s="2">
+        <f>B34*0.000001</f>
+        <v>9.1199999999999994E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3">
+        <f>B35*0.000001</f>
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="7">
+        <v>213.6</v>
+      </c>
+      <c r="C38" s="7">
+        <f>B38*0.000001</f>
+        <v>2.1359999999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="9">
+        <v>4</v>
+      </c>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="15">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B30+7+7)))</f>
+        <v>17.56910367703771</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="5">
+        <f>1/(C33+C34+(C32*(B36+3+B37+1+B31+B40+7+7)))</f>
+        <v>17.625773110473059</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="12">
+        <f>(C32*(3+B39+1+B31+B40+7+7)-C38+C33+C34+C35)/0.000001</f>
+        <v>56071</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>